<commit_message>
Code set for Frontend
</commit_message>
<xml_diff>
--- a/backend/DDF/ddf-transactions.xlsx
+++ b/backend/DDF/ddf-transactions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -668,6 +668,105 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>19</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Credit</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>committee@gmail.com</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2023-04-29 01:13:15</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1093.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>11.00</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Debit</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>faculty1@gmail.com</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2023-04-29 03:23:11</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1082.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>22</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>200.00</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Credit</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>committee@gmail.com</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2023-04-29 03:44:20</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1282.11</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>